<commit_message>
fix: Program.cs: Resolvendo problema no parse de valores da API (250.00 virava 25000 ao inves de 250)
(LG)
</commit_message>
<xml_diff>
--- a/Report_Generator_V1/bin/Debug/relatorio saude financeira.xlsx
+++ b/Report_Generator_V1/bin/Debug/relatorio saude financeira.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luiz-pc\Documents\HACKATHON\SafraHackathon\Report_Generator_V1\bin\Debug\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2F5F17D5-BB7C-43AC-90C4-BF630C53107F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7650E1CC-1DF8-4C57-89DF-DE47EBA5511A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9570" yWindow="3450" windowWidth="28800" windowHeight="11385" xr2:uid="{E3569B0D-4BC5-49A6-86FC-EC1A7143F00A}"/>
+    <workbookView xWindow="9600" yWindow="4140" windowWidth="28800" windowHeight="11385" xr2:uid="{37C0E382-FC01-40B4-A37C-EED69449E4FD}"/>
   </bookViews>
   <sheets>
     <sheet name="resumo_consolidado" sheetId="3" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
   <si>
     <t>RESUMO CONSOLIDADO DE PREVISÃO DE SAÚDE FINANCEIRA</t>
   </si>
@@ -47,10 +47,13 @@
     <t>EXECUTION TIME</t>
   </si>
   <si>
+    <t>Neutro</t>
+  </si>
+  <si>
     <t>Risco iminente de inadimplência</t>
   </si>
   <si>
-    <t>Investidor</t>
+    <t>Possível investidor</t>
   </si>
   <si>
     <t>Relação de Entrada (IN) e Saída (OUT) de contas PF Banco Safra</t>
@@ -297,6 +300,76 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
+                  <c:v>Neutro</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="3"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="F7DEDC"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>listagem_formulas!$H$3:$H$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>listagem_formulas!$I$3:$I$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>250</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000008-A629-434E-BFD4-76CC50ECB9CE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>listagem_formulas!$J$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
                   <c:v>Risco iminente de inadimplência</c:v>
                 </c:pt>
               </c:strCache>
@@ -334,22 +407,19 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>800000</c:v>
+                  <c:v>8000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>listagem_formulas!$I$3:$I$5</c:f>
+              <c:f>listagem_formulas!$J$3:$J$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>25000</c:v>
-                </c:pt>
                 <c:pt idx="1">
-                  <c:v>800000</c:v>
+                  <c:v>8000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -357,20 +427,20 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000008-2651-4016-8AD6-E9741797CB66}"/>
+              <c16:uniqueId val="{00000009-A629-434E-BFD4-76CC50ECB9CE}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
+          <c:idx val="2"/>
+          <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>listagem_formulas!$J$2</c:f>
+              <c:f>listagem_formulas!$K$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Investidor</c:v>
+                  <c:v>Possível investidor</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -386,7 +456,7 @@
             <c:size val="3"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="B58E41"/>
+                <a:srgbClr val="C9AF6D"/>
               </a:solidFill>
               <a:ln>
                 <a:noFill/>
@@ -407,19 +477,19 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>800000</c:v>
+                  <c:v>8000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>listagem_formulas!$J$3:$J$5</c:f>
+              <c:f>listagem_formulas!$K$3:$K$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="2">
-                  <c:v>25000</c:v>
+                  <c:v>250</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -427,7 +497,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000009-2651-4016-8AD6-E9741797CB66}"/>
+              <c16:uniqueId val="{0000000A-A629-434E-BFD4-76CC50ECB9CE}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -439,11 +509,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1179578736"/>
-        <c:axId val="1178503056"/>
+        <c:axId val="121000880"/>
+        <c:axId val="123752400"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1179578736"/>
+        <c:axId val="121000880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -547,12 +617,12 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1178503056"/>
+        <c:crossAx val="123752400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1178503056"/>
+        <c:axId val="123752400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -661,7 +731,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1179578736"/>
+        <c:crossAx val="121000880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -841,7 +911,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>listagem_formulas!$Q$2</c:f>
+              <c:f>listagem_formulas!$R$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -852,6 +922,30 @@
           </c:tx>
           <c:dPt>
             <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="F7DEDC"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000009-DF3E-4464-A538-C4EB71B7922B}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
@@ -870,16 +964,16 @@
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000009-E435-4C6E-8219-31F441FD7F84}"/>
+                <c16:uniqueId val="{0000000A-DF3E-4464-A538-C4EB71B7922B}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
           <c:dPt>
-            <c:idx val="1"/>
+            <c:idx val="2"/>
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="B58E41"/>
+                <a:srgbClr val="C9AF6D"/>
               </a:solidFill>
               <a:ln>
                 <a:noFill/>
@@ -894,7 +988,7 @@
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{0000000A-E435-4C6E-8219-31F441FD7F84}"/>
+                <c16:uniqueId val="{0000000B-DF3E-4464-A538-C4EB71B7922B}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -954,28 +1048,34 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>listagem_formulas!$P$3:$P$4</c:f>
+              <c:f>listagem_formulas!$Q$3:$Q$5</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
+                  <c:v>Neutro</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>Risco iminente de inadimplência</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>Investidor</c:v>
+                <c:pt idx="2">
+                  <c:v>Possível investidor</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>listagem_formulas!$Q$3:$Q$4</c:f>
+              <c:f>listagem_formulas!$R$3:$R$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0.66666666666666663</c:v>
+                  <c:v>0.33333333333333331</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>0.33333333333333331</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>0.33333333333333331</c:v>
                 </c:pt>
               </c:numCache>
@@ -983,7 +1083,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000008-E435-4C6E-8219-31F441FD7F84}"/>
+              <c16:uniqueId val="{00000008-DF3E-4464-A538-C4EB71B7922B}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2226,7 +2326,7 @@
         <xdr:cNvPr id="2" name="Gráfico 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2EF0E635-F674-4656-8B4E-CF21055A1D45}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E19CF516-98EC-43C0-B5F0-6EC362C4A78C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2262,7 +2362,7 @@
         <xdr:cNvPr id="3" name="Gráfico 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{898F69C0-1AB9-4B9F-ABFC-328E544F2AD6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E4412C75-1581-4885-A140-32CD59F8DFD8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2579,7 +2679,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78BE85DF-5CD6-4C03-8BFF-1B8634EB537F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0481BCEE-9C9E-4A21-ABD9-2720467BACDA}">
   <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -2730,17 +2830,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E6A55E0-F5E7-4D44-9B31-3B9D7F013D00}">
-  <dimension ref="A1:Q5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E55A5761-349C-4672-B503-C18E1DA7ABD8}">
+  <dimension ref="A1:R5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="8" max="10" width="12.7109375" customWidth="1"/>
+    <col min="8" max="11" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>1</v>
       </c>
@@ -2757,21 +2857,22 @@
         <v>5</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I1" s="8"/>
-      <c r="J1" s="9"/>
-      <c r="P1" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="Q1" s="9"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="9"/>
+      <c r="Q1" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="R1" s="9"/>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>711234511</v>
       </c>
       <c r="B2" s="5">
-        <v>25000</v>
+        <v>250</v>
       </c>
       <c r="C2" s="5">
         <v>0</v>
@@ -2780,10 +2881,10 @@
         <v>6</v>
       </c>
       <c r="E2" s="6">
-        <v>44087.722222222219</v>
+        <v>44087.787499999999</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I2" s="5" t="s">
         <v>6</v>
@@ -2791,93 +2892,105 @@
       <c r="J2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="P2" s="5" t="s">
-        <v>11</v>
+      <c r="K2" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="Q2" s="5" t="s">
         <v>12</v>
       </c>
+      <c r="R2" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>711234522</v>
       </c>
       <c r="B3" s="5">
-        <v>800000</v>
+        <v>8000</v>
       </c>
       <c r="C3" s="5">
         <v>0</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E3" s="6">
-        <v>44087.722222222219</v>
+        <v>44087.787499999999</v>
       </c>
       <c r="H3" s="5">
         <v>0</v>
       </c>
       <c r="I3" s="5">
-        <v>25000</v>
+        <v>250</v>
       </c>
       <c r="J3" s="5"/>
-      <c r="P3" s="5" t="s">
+      <c r="K3" s="5"/>
+      <c r="Q3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="Q3" s="5">
-        <v>0.66666666666666663</v>
+      <c r="R3" s="5">
+        <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>711234533</v>
       </c>
       <c r="B4" s="5">
-        <v>25000</v>
+        <v>250</v>
       </c>
       <c r="C4" s="5">
-        <v>800000</v>
+        <v>8000</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E4" s="6">
-        <v>44087.722222222219</v>
+        <v>44087.787499999999</v>
       </c>
       <c r="H4" s="5">
         <v>0</v>
       </c>
-      <c r="I4" s="5">
-        <v>800000</v>
-      </c>
-      <c r="J4" s="5"/>
-      <c r="P4" s="5" t="s">
+      <c r="I4" s="5"/>
+      <c r="J4" s="5">
+        <v>8000</v>
+      </c>
+      <c r="K4" s="5"/>
+      <c r="Q4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="Q4" s="5">
+      <c r="R4" s="5">
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="H5" s="5">
-        <v>800000</v>
+        <v>8000</v>
       </c>
       <c r="I5" s="5"/>
-      <c r="J5" s="5">
-        <v>25000</v>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5">
+        <v>250</v>
+      </c>
+      <c r="Q5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="R5" s="5">
+        <v>0.33333333333333331</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="H1:J1"/>
-    <mergeCell ref="P1:Q1"/>
+    <mergeCell ref="H1:K1"/>
+    <mergeCell ref="Q1:R1"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE73C4DF-5B9D-40EB-A1F0-125E9B106246}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DADD029-5355-4A6B-9526-6FFB73642D16}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>